<commit_message>
Improve depth and width of tree
</commit_message>
<xml_diff>
--- a/Temat11/AllData/ComparingExecutionTime.xlsx
+++ b/Temat11/AllData/ComparingExecutionTime.xlsx
@@ -43,9 +43,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -86,32 +86,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,8 +110,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,13 +127,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,7 +165,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,7 +180,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,12 +217,108 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -235,25 +331,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,139 +391,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,41 +408,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -485,6 +450,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -508,20 +488,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -534,127 +534,127 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -778,10 +778,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pl-PL" altLang="en-US"/>
               <a:t>Executing time of query:</a:t>
             </a:r>
-            <a:endParaRPr lang="pl-PL" altLang="en-US"/>
           </a:p>
           <a:p>
             <a:pPr defTabSz="914400">
@@ -798,491 +796,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pl-PL" altLang="en-US" sz="1200" b="1"/>
-              <a:t>select * from person</a:t>
-            </a:r>
-            <a:endParaRPr lang="pl-PL" altLang="en-US" sz="1200" b="1"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SINGLE_TABLE</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$4:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$4:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>970</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1020</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>953</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>935</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TABLE_PER_CLASS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$4:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$4:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>765</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>796</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>812</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>755</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>771</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>JOINED</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="0070C0"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$4:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$4:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>972</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>988</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>970</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>965</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>954</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="698455354"/>
-        <c:axId val="442827146"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="698455354"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="442827146"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="442827146"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="698455354"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr lang="en-US"/>
-      </a:pPr>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr defTabSz="914400">
-              <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:t>Executing time of query:-</a:t>
-            </a:r>
-            <a:r>
               <a:rPr sz="1200" b="1"/>
               <a:t>select * from person</a:t>
             </a:r>
+            <a:endParaRPr sz="1200" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1408,7 +925,7 @@
             </a:solidFill>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="92D050"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -1424,7 +941,7 @@
               </a:solidFill>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="F85208"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1879,46 +1396,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2422,541 +1899,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>71120</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>116840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>116840</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="71120" y="2860040"/>
-        <a:ext cx="5143500" cy="2743200"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -2981,7 +1925,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3251,7 +2195,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>

</xml_diff>